<commit_message>
rnc-22/02/2015-Se agregaron las bitácoras pertenecientes a la semana 2 y 3
</commit_message>
<xml_diff>
--- a/ afgmx/AFGMX/ADMON_DEL_PROYECTO/BITACORAS/2015/FEB/bitacora.xlsx
+++ b/ afgmx/AFGMX/ADMON_DEL_PROYECTO/BITACORAS/2015/FEB/bitacora.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="65">
   <si>
     <t>UNIVERSIDAD TECNOLÓGICA DEL  CENTRO DE VERACRUZ
 TECNOLOGÍAS DE LA INFORMACIÓN Y COMUNICACIÓN
@@ -199,14 +199,36 @@
   </si>
   <si>
     <t>Verificación de nuevas actividades e integración de procesos</t>
+  </si>
+  <si>
+    <t>02/18/2015</t>
+  </si>
+  <si>
+    <t>Finalizado</t>
+  </si>
+  <si>
+    <t>Elaboración de documento del proceso</t>
+  </si>
+  <si>
+    <t>Documento del proceso</t>
+  </si>
+  <si>
+    <t>Se llevo a cabo la elaboración del documento del proceso, para lo cual se  subdividió el trabajo entre los integrantes del equipo, al final se verifico entre todos que lo definido en las actividades estuviera bien redactado. De igual forma se programo una pr´xima reunión el día martes 22 del mes en curso.</t>
+  </si>
+  <si>
+    <t>Corrección de repositorio</t>
+  </si>
+  <si>
+    <t>La reunión fue con el motivo de ver la correcta estructura del repositorio y ver que integrantes del equipo debían añadir correcciones tanto al orden como al nombre de los archivos se acordó como fecha limite el día 16 del mes en curso.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="d/m/yy;@"/>
   </numFmts>
   <fonts count="56" x14ac:knownFonts="1">
     <font>
@@ -1226,7 +1248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1300,6 +1322,27 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="22" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1318,27 +1361,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="22" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1348,6 +1370,24 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1375,23 +1415,8 @@
     <xf numFmtId="0" fontId="12" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1872,7 +1897,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1912,46 +1937,46 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="39"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="46"/>
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="39"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="46"/>
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="39"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="46"/>
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1974,13 +1999,13 @@
       <c r="C6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
@@ -1992,13 +2017,13 @@
       <c r="C7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
@@ -2010,13 +2035,13 @@
       <c r="C8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
@@ -2028,13 +2053,13 @@
       <c r="C9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
       <c r="I9" s="15"/>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
@@ -2046,13 +2071,13 @@
       <c r="C10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="43">
+      <c r="D10" s="39">
         <v>1</v>
       </c>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
@@ -2064,13 +2089,13 @@
       <c r="C11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="46" t="s">
+      <c r="D11" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
@@ -2096,11 +2121,11 @@
       <c r="C13" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
       <c r="I13" s="15"/>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
@@ -2112,13 +2137,13 @@
       <c r="C14" s="26">
         <v>1</v>
       </c>
-      <c r="D14" s="48" t="s">
+      <c r="D14" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
@@ -2130,13 +2155,13 @@
       <c r="C15" s="26">
         <v>2</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="D15" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
@@ -2148,13 +2173,13 @@
       <c r="C16" s="26">
         <v>3</v>
       </c>
-      <c r="D16" s="44" t="s">
+      <c r="D16" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
       <c r="I16" s="15"/>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
@@ -2166,13 +2191,13 @@
       <c r="C17" s="26">
         <v>4</v>
       </c>
-      <c r="D17" s="44" t="s">
+      <c r="D17" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
@@ -2184,13 +2209,13 @@
       <c r="C18" s="26">
         <v>5</v>
       </c>
-      <c r="D18" s="44" t="s">
+      <c r="D18" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
@@ -2202,11 +2227,11 @@
       <c r="C19" s="26">
         <v>6</v>
       </c>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
@@ -2228,6 +2253,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B2:K4"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="D9:H9"/>
     <mergeCell ref="D16:H16"/>
     <mergeCell ref="D17:H17"/>
     <mergeCell ref="D18:H18"/>
@@ -2237,11 +2267,6 @@
     <mergeCell ref="D13:H13"/>
     <mergeCell ref="D14:H14"/>
     <mergeCell ref="D15:H15"/>
-    <mergeCell ref="B2:K4"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="D9:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2253,7 +2278,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2420,26 +2445,54 @@
     </row>
     <row r="10" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="36"/>
+      <c r="B10" s="22">
+        <v>2</v>
+      </c>
+      <c r="C10" s="11">
+        <v>42310</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>54</v>
+      </c>
       <c r="I10" s="13"/>
       <c r="J10" s="2"/>
       <c r="K10" s="15"/>
     </row>
     <row r="11" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="22"/>
+      <c r="B11" s="22">
+        <v>3</v>
+      </c>
+      <c r="C11" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="36" t="s">
+        <v>54</v>
+      </c>
       <c r="I11" s="13"/>
       <c r="J11" s="2"/>
       <c r="K11" s="15"/>
@@ -2753,10 +2806,10 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="53"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -2780,10 +2833,10 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="53"/>
+      <c r="C7" s="59"/>
       <c r="D7" s="34"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -2828,44 +2881,44 @@
     </row>
     <row r="9" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="55"/>
-      <c r="E9" s="56" t="s">
+      <c r="D9" s="61"/>
+      <c r="E9" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="57" t="s">
+      <c r="F9" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="59" t="s">
+      <c r="G9" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="60"/>
-      <c r="N9" s="60"/>
-      <c r="O9" s="60"/>
-      <c r="P9" s="60"/>
-      <c r="Q9" s="60"/>
-      <c r="R9" s="60"/>
-      <c r="S9" s="60"/>
-      <c r="T9" s="60"/>
-      <c r="U9" s="61"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="66"/>
+      <c r="N9" s="66"/>
+      <c r="O9" s="66"/>
+      <c r="P9" s="66"/>
+      <c r="Q9" s="66"/>
+      <c r="R9" s="66"/>
+      <c r="S9" s="66"/>
+      <c r="T9" s="66"/>
+      <c r="U9" s="67"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
-      <c r="B10" s="54"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="58"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="64"/>
       <c r="G10" s="23">
         <v>1</v>
       </c>
@@ -2914,12 +2967,12 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
-      <c r="B11" s="62">
+      <c r="B11" s="53">
         <v>1</v>
       </c>
-      <c r="C11" s="63"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="66"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="56"/>
       <c r="F11" s="25" t="s">
         <v>27</v>
       </c>
@@ -2941,10 +2994,10 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
-      <c r="B12" s="62"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="67"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="57"/>
       <c r="F12" s="25" t="s">
         <v>28</v>
       </c>
@@ -2966,12 +3019,12 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
-      <c r="B13" s="62">
+      <c r="B13" s="53">
         <v>2</v>
       </c>
-      <c r="C13" s="65"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="66"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="56"/>
       <c r="F13" s="25" t="s">
         <v>27</v>
       </c>
@@ -2993,10 +3046,10 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
-      <c r="B14" s="62"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="67"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="57"/>
       <c r="F14" s="25" t="s">
         <v>28</v>
       </c>
@@ -3018,12 +3071,12 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="20"/>
-      <c r="B15" s="62">
+      <c r="B15" s="53">
         <v>3</v>
       </c>
-      <c r="C15" s="63"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="66"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="56"/>
       <c r="F15" s="25" t="s">
         <v>27</v>
       </c>
@@ -3045,10 +3098,10 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="67"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="57"/>
       <c r="F16" s="25" t="s">
         <v>28</v>
       </c>
@@ -3070,12 +3123,12 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
-      <c r="B17" s="62">
+      <c r="B17" s="53">
         <v>4</v>
       </c>
-      <c r="C17" s="63"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="66"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="56"/>
       <c r="F17" s="25" t="s">
         <v>27</v>
       </c>
@@ -3097,10 +3150,10 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
-      <c r="B18" s="62"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="67"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="57"/>
       <c r="F18" s="25" t="s">
         <v>28</v>
       </c>
@@ -3122,12 +3175,12 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="20"/>
-      <c r="B19" s="62">
+      <c r="B19" s="53">
         <v>5</v>
       </c>
-      <c r="C19" s="65"/>
-      <c r="D19" s="64"/>
-      <c r="E19" s="66"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="56"/>
       <c r="F19" s="25" t="s">
         <v>27</v>
       </c>
@@ -3149,10 +3202,10 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
-      <c r="B20" s="62"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="67"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="57"/>
       <c r="F20" s="25" t="s">
         <v>28</v>
       </c>
@@ -3174,12 +3227,12 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="20"/>
-      <c r="B21" s="62">
+      <c r="B21" s="53">
         <v>6</v>
       </c>
-      <c r="C21" s="63"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="66"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="56"/>
       <c r="F21" s="25" t="s">
         <v>27</v>
       </c>
@@ -3201,10 +3254,10 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
-      <c r="B22" s="62"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="67"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="57"/>
       <c r="F22" s="25" t="s">
         <v>28</v>
       </c>
@@ -3226,12 +3279,12 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="20"/>
-      <c r="B23" s="62">
+      <c r="B23" s="53">
         <v>7</v>
       </c>
-      <c r="C23" s="65"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="66"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="56"/>
       <c r="F23" s="25" t="s">
         <v>27</v>
       </c>
@@ -3253,10 +3306,10 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
-      <c r="B24" s="62"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="67"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="57"/>
       <c r="F24" s="25" t="s">
         <v>28</v>
       </c>
@@ -3278,12 +3331,12 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
-      <c r="B25" s="62">
+      <c r="B25" s="53">
         <v>8</v>
       </c>
-      <c r="C25" s="65"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="66"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="56"/>
       <c r="F25" s="25" t="s">
         <v>27</v>
       </c>
@@ -3305,10 +3358,10 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
-      <c r="B26" s="62"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="67"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="57"/>
       <c r="F26" s="25" t="s">
         <v>28</v>
       </c>
@@ -3330,12 +3383,12 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="20"/>
-      <c r="B27" s="62">
+      <c r="B27" s="53">
         <v>9</v>
       </c>
-      <c r="C27" s="65"/>
-      <c r="D27" s="64"/>
-      <c r="E27" s="66"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="56"/>
       <c r="F27" s="25" t="s">
         <v>27</v>
       </c>
@@ -3357,10 +3410,10 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
-      <c r="B28" s="62"/>
-      <c r="C28" s="65"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="67"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="57"/>
       <c r="F28" s="25" t="s">
         <v>28</v>
       </c>
@@ -3382,12 +3435,12 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="20"/>
-      <c r="B29" s="62">
+      <c r="B29" s="53">
         <v>10</v>
       </c>
-      <c r="C29" s="65"/>
-      <c r="D29" s="64"/>
-      <c r="E29" s="66"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="56"/>
       <c r="F29" s="25" t="s">
         <v>27</v>
       </c>
@@ -3409,10 +3462,10 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
-      <c r="B30" s="62"/>
-      <c r="C30" s="65"/>
-      <c r="D30" s="64"/>
-      <c r="E30" s="67"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="57"/>
       <c r="F30" s="25" t="s">
         <v>28</v>
       </c>
@@ -3434,12 +3487,12 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="20"/>
-      <c r="B31" s="62">
+      <c r="B31" s="53">
         <v>11</v>
       </c>
-      <c r="C31" s="65"/>
-      <c r="D31" s="64"/>
-      <c r="E31" s="66"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="56"/>
       <c r="F31" s="25" t="s">
         <v>27</v>
       </c>
@@ -3461,10 +3514,10 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
-      <c r="B32" s="62"/>
-      <c r="C32" s="65"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="67"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="57"/>
       <c r="F32" s="25" t="s">
         <v>28</v>
       </c>
@@ -3486,12 +3539,12 @@
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="20"/>
-      <c r="B33" s="62">
+      <c r="B33" s="53">
         <v>12</v>
       </c>
-      <c r="C33" s="65"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="66"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="56"/>
       <c r="F33" s="25" t="s">
         <v>27</v>
       </c>
@@ -3513,10 +3566,10 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="15"/>
-      <c r="B34" s="62"/>
-      <c r="C34" s="65"/>
-      <c r="D34" s="64"/>
-      <c r="E34" s="67"/>
+      <c r="B34" s="53"/>
+      <c r="C34" s="54"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="57"/>
       <c r="F34" s="25" t="s">
         <v>28</v>
       </c>
@@ -3538,12 +3591,12 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="20"/>
-      <c r="B35" s="62">
+      <c r="B35" s="53">
         <v>13</v>
       </c>
-      <c r="C35" s="65"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="66"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="56"/>
       <c r="F35" s="25" t="s">
         <v>27</v>
       </c>
@@ -3565,10 +3618,10 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
-      <c r="B36" s="62"/>
-      <c r="C36" s="65"/>
-      <c r="D36" s="64"/>
-      <c r="E36" s="67"/>
+      <c r="B36" s="53"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="57"/>
       <c r="F36" s="25" t="s">
         <v>28</v>
       </c>
@@ -3590,12 +3643,12 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="20"/>
-      <c r="B37" s="62">
+      <c r="B37" s="53">
         <v>14</v>
       </c>
-      <c r="C37" s="65"/>
-      <c r="D37" s="64"/>
-      <c r="E37" s="66"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="56"/>
       <c r="F37" s="25" t="s">
         <v>27</v>
       </c>
@@ -3617,10 +3670,10 @@
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
-      <c r="B38" s="62"/>
-      <c r="C38" s="65"/>
-      <c r="D38" s="64"/>
-      <c r="E38" s="67"/>
+      <c r="B38" s="53"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="55"/>
+      <c r="E38" s="57"/>
       <c r="F38" s="25" t="s">
         <v>28</v>
       </c>
@@ -3642,12 +3695,12 @@
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="20"/>
-      <c r="B39" s="62">
+      <c r="B39" s="53">
         <v>15</v>
       </c>
-      <c r="C39" s="65"/>
-      <c r="D39" s="64"/>
-      <c r="E39" s="66"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="56"/>
       <c r="F39" s="25" t="s">
         <v>27</v>
       </c>
@@ -3669,10 +3722,10 @@
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
-      <c r="B40" s="62"/>
-      <c r="C40" s="65"/>
-      <c r="D40" s="64"/>
-      <c r="E40" s="67"/>
+      <c r="B40" s="53"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="55"/>
+      <c r="E40" s="57"/>
       <c r="F40" s="25" t="s">
         <v>28</v>
       </c>
@@ -3694,6 +3747,50 @@
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="B2:U4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:U9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:D34"/>
+    <mergeCell ref="E33:E34"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="C39:D40"/>
     <mergeCell ref="E39:E40"/>
@@ -3703,50 +3800,6 @@
     <mergeCell ref="B37:B38"/>
     <mergeCell ref="C37:D38"/>
     <mergeCell ref="E37:E38"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="B2:U4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:U9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>